<commit_message>
remove type as field
</commit_message>
<xml_diff>
--- a/example/transactions.xlsx
+++ b/example/transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Desktop/fifo_calculator/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Nextcloud/pyFIFOtax/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94196DB3-E326-D24C-A832-C7D284845868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70F07B-3D65-FE44-845A-26FA0D748B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2220" windowWidth="51200" windowHeight="23440" xr2:uid="{258DE83D-C90A-AA43-91A0-3CBCDC3341E2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{258DE83D-C90A-AA43-91A0-3CBCDC3341E2}"/>
   </bookViews>
   <sheets>
     <sheet name="deposits" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
   <si>
     <t>NVDA</t>
   </si>
@@ -57,15 +57,6 @@
   </si>
   <si>
     <t>tax_withholding</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>RSU</t>
-  </si>
-  <si>
-    <t>ESPP</t>
   </si>
   <si>
     <t>quantity</t>
@@ -461,7 +452,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,17 +472,15 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -504,13 +493,10 @@
         <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,13 +510,10 @@
         <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -544,13 +527,10 @@
         <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -564,18 +544,15 @@
         <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>43749</v>
@@ -584,18 +561,15 @@
         <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>44845</v>
@@ -604,13 +578,10 @@
         <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -664,12 +635,12 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>44743</v>
@@ -681,7 +652,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -710,16 +681,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -739,7 +710,7 @@
         <v>0.03</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -759,7 +730,7 @@
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -779,7 +750,7 @@
         <v>0.01</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -799,12 +770,12 @@
         <v>0.02</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>44867</v>
@@ -819,12 +790,12 @@
         <v>0.01</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>44868</v>
@@ -839,12 +810,12 @@
         <v>0.01</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>44868</v>
@@ -859,12 +830,12 @@
         <v>0.01</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>44879</v>
@@ -879,7 +850,7 @@
         <v>0.01</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -906,13 +877,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -926,7 +897,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -940,7 +911,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
treat wire transfers only optionally as exchanges, address some further feedback
</commit_message>
<xml_diff>
--- a/example/transactions.xlsx
+++ b/example/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/pyFIFOtax/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856866E8-62E6-5747-BB70-9BCD748178AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62829B7B-0EDB-4741-B204-CF1359D18E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rsu" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -1007,13 +1007,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413B3602-8121-5942-A389-F7BB3F804A41}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1024,13 +1024,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>45292</v>
       </c>
@@ -1040,12 +1043,15 @@
       <c r="C2" s="7">
         <v>100</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>45293</v>
       </c>
@@ -1055,11 +1061,14 @@
       <c r="C3">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>45294</v>
       </c>
@@ -1067,13 +1076,16 @@
         <v>45294</v>
       </c>
       <c r="C4">
-        <v>-100</v>
-      </c>
-      <c r="D4" t="s">
+        <v>-98</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>45294</v>
       </c>
@@ -1081,9 +1093,12 @@
         <v>45294</v>
       </c>
       <c r="C5">
-        <v>-100</v>
-      </c>
-      <c r="D5" t="s">
+        <v>-98</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rename currency movements to money transfers
</commit_message>
<xml_diff>
--- a/example/transactions.xlsx
+++ b/example/transactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/pyFIFOtax/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62829B7B-0EDB-4741-B204-CF1359D18E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B52C18E-DF11-204C-9EA0-584E23312CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="buy_orders" sheetId="5" r:id="rId4"/>
     <sheet name="sell_orders" sheetId="3" r:id="rId5"/>
     <sheet name="currency_conversions" sheetId="4" r:id="rId6"/>
-    <sheet name="currency_movements" sheetId="10" r:id="rId7"/>
+    <sheet name="money_transfers" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>

</xml_diff>

<commit_message>
refactor currency conversion, now explicit source and target amounts
</commit_message>
<xml_diff>
--- a/example/transactions.xlsx
+++ b/example/transactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mstadler/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/pyFIFOtax/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB081B3-1753-774D-A4FF-F1E4813CEB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC07B6D8-DB91-A545-A9DD-0E3A73D47775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rsu" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -101,9 +101,6 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>foreign_amount</t>
-  </si>
-  <si>
     <t>source_fees</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>buy_date</t>
+  </si>
+  <si>
+    <t>target_fees</t>
+  </si>
+  <si>
+    <t>source_amount</t>
+  </si>
+  <si>
+    <t>target_amount</t>
   </si>
 </sst>
 </file>
@@ -409,7 +415,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -570,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -647,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="3"/>
     </row>
@@ -722,7 +728,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -933,9 +939,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -943,27 +949,33 @@
     <col min="2" max="16384" width="16.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>44846</v>
       </c>
@@ -976,11 +988,17 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>44896</v>
       </c>
@@ -993,7 +1011,13 @@
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1007,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413B3602-8121-5942-A389-F7BB3F804A41}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1016,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>9</v>
@@ -1028,7 +1052,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>